<commit_message>
imporved citation seciton detection algorithm
</commit_message>
<xml_diff>
--- a/python/data/vas_top50_most_rel_overcites_new.xlsx
+++ b/python/data/vas_top50_most_rel_overcites_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\workspace\academicFraudDetector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\workspace\academicFraudDetector\python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3949,11 +3949,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1670"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A901" workbookViewId="0">
-      <selection activeCell="H835" sqref="H835"/>
+    <sheetView tabSelected="1" topLeftCell="A1343" workbookViewId="0">
+      <selection activeCell="B1361" sqref="B1361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="124.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -14031,7 +14034,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="956" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="956" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A956" s="1" t="s">
         <v>36</v>
       </c>
@@ -14390,7 +14393,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="990" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="990" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A990" s="1" t="s">
         <v>36</v>
       </c>
@@ -14749,7 +14752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="1024" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1024" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1024" s="1" t="s">
         <v>36</v>
       </c>
@@ -15108,7 +15111,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="1058" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1058" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1058" s="1" t="s">
         <v>36</v>
       </c>
@@ -15467,7 +15470,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="1092" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1092" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1092" s="1" t="s">
         <v>36</v>
       </c>
@@ -15826,7 +15829,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="1126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1126" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1126" s="1" t="s">
         <v>36</v>
       </c>
@@ -16185,7 +16188,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="1160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1160" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1160" s="1" t="s">
         <v>36</v>
       </c>
@@ -16544,7 +16547,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1194" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1194" s="1" t="s">
         <v>36</v>
       </c>
@@ -16903,7 +16906,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="1228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1228" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1228" s="1" t="s">
         <v>36</v>
       </c>
@@ -17262,7 +17265,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="1262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1262" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1262" s="1" t="s">
         <v>36</v>
       </c>
@@ -17621,7 +17624,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="1296" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1296" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1296" s="1" t="s">
         <v>36</v>
       </c>
@@ -17980,7 +17983,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="1330" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1330" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1330" s="1" t="s">
         <v>36</v>
       </c>
@@ -18339,7 +18342,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1364" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1364" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1364" s="1" t="s">
         <v>36</v>
       </c>
@@ -18698,7 +18701,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="1398" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1398" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1398" s="1" t="s">
         <v>36</v>
       </c>
@@ -19057,7 +19060,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="1432" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1432" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1432" s="1" t="s">
         <v>36</v>
       </c>
@@ -19416,7 +19419,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1466" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1466" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1466" s="1" t="s">
         <v>36</v>
       </c>
@@ -19775,7 +19778,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="1500" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1500" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1500" s="1" t="s">
         <v>36</v>
       </c>
@@ -20134,7 +20137,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="1534" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1534" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1534" s="1" t="s">
         <v>36</v>
       </c>
@@ -20493,7 +20496,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="1568" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1568" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1568" s="1" t="s">
         <v>36</v>
       </c>
@@ -20852,7 +20855,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="1602" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1602" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1602" s="1" t="s">
         <v>36</v>
       </c>
@@ -21211,7 +21214,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="1636" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1636" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1636" s="1" t="s">
         <v>36</v>
       </c>
@@ -21570,7 +21573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1670" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1670" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1670" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>